<commit_message>
Corrected spelling mistake and removed unecessary fields used for testing.
</commit_message>
<xml_diff>
--- a/Notification List.xlsx
+++ b/Notification List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keert\source\repos\excelToWhatsapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arul/PycharmProjects/excelToWhatsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6403A13F-A417-4398-BE6D-160E1F598FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378BE7DA-ECAC-4147-BFBD-5717F9765A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="3825" windowWidth="32175" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="3820" windowWidth="39840" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Event Type</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Event Template Example</t>
+  </si>
+  <si>
+    <t>Event Types</t>
+  </si>
+  <si>
+    <t>First Message</t>
   </si>
   <si>
     <t>Sri Srinivasa Perumal Temple :
@@ -81,7 +87,7 @@
 Date : [Date]
 Time : [Time]
 Please do not reply to this message.
-For any queruies, please call the 
+For any queries, please call the 
 Temple Office at 6298 5771</t>
   </si>
   <si>
@@ -91,40 +97,15 @@
 Date : 21 May 2022
 Time : 8.30 am
 Please do not reply to this message.
-For any queruies, please call the 
+For any queries, please call the 
 Temple Office at 6298 5771</t>
-  </si>
-  <si>
-    <t>Sri Srinivasa Perumal Temple :
-0.0
-Reminder
-[EventType] : [EventName]
-Date : [Date]
-Time : [Time]
-Please do not reply to this message.
-For any queruies, please call the 
-Temple Office at 6298 5771</t>
-  </si>
-  <si>
-    <t>Sri Srinivasa Perumal Temple :
-Reminder
-Ubaya : Mahalakshmi Kuberayagam
-Date : 21 May 2022
-Time : 8.30 am
-Please do not reply to this message.
-For any queruies, please call the 
-Temple Office at 6298 5771</t>
-  </si>
-  <si>
-    <t>Event Types</t>
-  </si>
-  <si>
-    <t>First Message</t>
   </si>
   <si>
     <t>Sri Srinivasa Perumal Temple:
 Dear SSPT devotee,
-We have embarked on a new initiative to inform you via WhatsApp on key SSPT specific events and your ubayams &amp; services at the temple. This is one our efforts to improve our engagement with you. We seek you understanding while we finetune the initiative. Looking forward to your support and constructive feedback.
+We have embarked on a new initiative to inform you via WhatsApp on key SSPT specific events and your ubayams &amp; services at the temple. 
+This is one our efforts to improve our engagement with you. We seek you understanding while we finetune the initiative. 
+Looking forward to your support and constructive feedback.
 Please do not reply to this message.
 For any queries, please call the
 Temple Office at 6298 5771</t>
@@ -568,19 +549,19 @@
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -630,7 +611,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -674,21 +655,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" customWidth="1"/>
-    <col min="4" max="4" width="93.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="93.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -699,34 +680,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="141" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="141" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="238" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="204" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -739,20 +709,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -761,7 +731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -772,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D3" t="s">
         <v>12</v>
       </c>

</xml_diff>